<commit_message>
almost everything done for 3sem
</commit_message>
<xml_diff>
--- a/ter-ver/2/Lab2.xlsx
+++ b/ter-ver/2/Lab2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2EAE31-E12B-4268-B32F-7EB44D47A2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F1E572-9507-4FFD-807D-B4E91DB67924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="294" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,8 +28,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>xi</t>
   </si>
@@ -131,6 +153,30 @@
   </si>
   <si>
     <t>r =</t>
+  </si>
+  <si>
+    <t>y = b0 + b1lnx</t>
+  </si>
+  <si>
+    <t>R^2 =</t>
+  </si>
+  <si>
+    <t>xy</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -481,6 +527,9 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -510,9 +559,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -911,6 +957,110 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>логарифмическая</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$D$29:$D$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$Z$26:$Z$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.583333333333329</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.344594323608192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.129753459065466</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.105855313883055</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.638638993743758</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.891014449340325</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.949882809582327</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-07AE-4ED1-B7BD-98FA2B658FF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1208,6 +1358,14 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="6"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
@@ -1215,7 +1373,7 @@
           <c:x val="0.81081113895738643"/>
           <c:y val="0.64448227242380063"/>
           <c:w val="0.18918888173650811"/>
-          <c:h val="0.26903978653972532"/>
+          <c:h val="0.2241998221164378"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3821,6 +3979,99 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>321324</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>192795</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>569204</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>174433</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54329A4B-1468-425B-9717-947AF6886EA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13348770" y="2579783"/>
+          <a:ext cx="1459735" cy="587566"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>y</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> = 12,5833 + 6,869 *lnx</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>R = 0,918367</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1000">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4087,10 +4338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:AI58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4100,12 +4351,13 @@
     <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="59"/>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
+      <c r="A1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
@@ -4341,6 +4593,9 @@
         <f t="shared" si="2"/>
         <v>3600</v>
       </c>
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="39">
@@ -4421,7 +4676,7 @@
       <c r="E16" s="48"/>
       <c r="F16" s="48"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" s="47" t="s">
         <v>33</v>
       </c>
@@ -4444,14 +4699,14 @@
         <v>2.4469118511449697</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="55" t="s">
+    <row r="18" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <f>B16</f>
         <v>8</v>
@@ -4466,7 +4721,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <f>A15</f>
         <v>28</v>
@@ -4481,19 +4736,19 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="64" t="s">
+    <row r="21" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="64"/>
-      <c r="C21" s="62" t="s">
+      <c r="B21" s="65"/>
+      <c r="C21" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" s="41">
         <f t="array" ref="A22:B23">MINVERSE(A19:B20)</f>
         <v>0.41666666666666663</v>
@@ -4512,7 +4767,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="43">
         <v>-8.3333333333333329E-2</v>
       </c>
@@ -4526,16 +4781,88 @@
         <v>6.8690476190476204</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="55" t="s">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="Z25" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A26" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="Z26" t="e">
+        <f>$D$22+$D$23*LN(D29)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AC26">
+        <f>C29*D29</f>
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <f>1/$B$16 * SUM(AC26:AC33)</f>
+        <v>164.25</v>
+      </c>
+      <c r="AE26">
+        <f>1/$B$16 * SUM(D29:D36)</f>
+        <v>3.5</v>
+      </c>
+      <c r="AF26">
+        <f>1/$B$16 *SUM(C29:C36)</f>
+        <v>36.625</v>
+      </c>
+      <c r="AG26" cm="1">
+        <f t="array" ref="AG26">1/$B$16 * SUM(D29:D36 * D29:D36) - $AE$26 ^ 2</f>
+        <v>5.25</v>
+      </c>
+      <c r="AH26">
+        <f>(AD26-AE26*AF26)/SQRT(AG26*AG27)</f>
+        <v>0.95831443629501956</v>
+      </c>
+      <c r="AI26">
+        <f>AH26^2</f>
+        <v>0.91836655881144114</v>
+      </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="Z27">
+        <f t="shared" ref="Z27:Z33" si="6">$D$22+$D$23*LN(D30)</f>
+        <v>12.583333333333329</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC27">
+        <f t="shared" ref="AC27:AC33" si="7">C30*D30</f>
+        <v>21</v>
+      </c>
+      <c r="AG27" cm="1">
+        <f t="array" ref="AG27">1/$B$16 * SUM(C29:C36 ^2) - $AF$26 ^ 2</f>
+        <v>269.734375</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="C28" s="5" t="s">
         <v>12</v>
@@ -4546,128 +4873,176 @@
       <c r="E28" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="Z28">
+        <f t="shared" si="6"/>
+        <v>17.344594323608192</v>
+      </c>
+      <c r="AC28">
+        <f t="shared" si="7"/>
+        <v>46</v>
+      </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
-      <c r="C29" s="65">
-        <f>B6</f>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A29" s="55"/>
+      <c r="C29" s="55">
+        <f t="shared" ref="C29:C36" si="8">B6</f>
         <v>19</v>
       </c>
-      <c r="D29" s="65">
-        <f t="shared" ref="D29:D36" si="6">A6</f>
+      <c r="D29" s="55">
+        <f t="shared" ref="D29:D36" si="9">A6</f>
         <v>0</v>
       </c>
-      <c r="E29" s="65">
-        <f t="shared" ref="E29:E36" si="7">1/B6</f>
+      <c r="E29" s="55">
+        <f t="shared" ref="E29:E36" si="10">1/B6</f>
         <v>5.2631578947368418E-2</v>
       </c>
+      <c r="Z29">
+        <f t="shared" si="6"/>
+        <v>20.129753459065466</v>
+      </c>
+      <c r="AC29">
+        <f t="shared" si="7"/>
+        <v>84</v>
+      </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
-      <c r="C30" s="65">
-        <f>B7</f>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A30" s="55"/>
+      <c r="C30" s="55">
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
-      <c r="D30" s="65">
+      <c r="D30" s="55">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="55">
+        <f t="shared" si="10"/>
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="Z30">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E30" s="65">
+        <v>22.105855313883055</v>
+      </c>
+      <c r="AC30">
         <f t="shared" si="7"/>
-        <v>4.7619047619047616E-2</v>
+        <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="65"/>
-      <c r="C31" s="65">
-        <f>B8</f>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A31" s="55"/>
+      <c r="C31" s="55">
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
-      <c r="D31" s="65">
+      <c r="D31" s="55">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="E31" s="55">
+        <f t="shared" si="10"/>
+        <v>4.3478260869565216E-2</v>
+      </c>
+      <c r="Z31">
         <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="E31" s="65">
+        <v>23.638638993743758</v>
+      </c>
+      <c r="AC31">
         <f t="shared" si="7"/>
-        <v>4.3478260869565216E-2</v>
+        <v>230</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
-      <c r="C32" s="65">
-        <f>B9</f>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A32" s="55"/>
+      <c r="C32" s="55">
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
-      <c r="D32" s="65">
+      <c r="D32" s="55">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="E32" s="55">
+        <f t="shared" si="10"/>
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="Z32">
         <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="E32" s="65">
+        <v>24.891014449340325</v>
+      </c>
+      <c r="AC32">
         <f t="shared" si="7"/>
-        <v>3.5714285714285712E-2</v>
+        <v>360</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="65"/>
-      <c r="C33" s="65">
-        <f>B10</f>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A33" s="55"/>
+      <c r="C33" s="55">
+        <f t="shared" si="8"/>
         <v>33</v>
       </c>
-      <c r="D33" s="65">
+      <c r="D33" s="55">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="E33" s="55">
+        <f t="shared" si="10"/>
+        <v>3.0303030303030304E-2</v>
+      </c>
+      <c r="Z33">
         <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="E33" s="65">
+        <v>25.949882809582327</v>
+      </c>
+      <c r="AC33">
         <f t="shared" si="7"/>
-        <v>3.0303030303030304E-2</v>
+        <v>441</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="65"/>
-      <c r="C34" s="65">
-        <f>B11</f>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A34" s="55"/>
+      <c r="C34" s="55">
+        <f t="shared" si="8"/>
         <v>46</v>
       </c>
-      <c r="D34" s="65">
-        <f t="shared" si="6"/>
+      <c r="D34" s="55">
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="E34" s="65">
-        <f t="shared" si="7"/>
+      <c r="E34" s="55">
+        <f t="shared" si="10"/>
         <v>2.1739130434782608E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="65"/>
-      <c r="C35" s="65">
-        <f>B12</f>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A35" s="55"/>
+      <c r="C35" s="55">
+        <f t="shared" si="8"/>
         <v>60</v>
       </c>
-      <c r="D35" s="65">
-        <f t="shared" si="6"/>
+      <c r="D35" s="55">
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
-      <c r="E35" s="65">
-        <f t="shared" si="7"/>
+      <c r="E35" s="55">
+        <f t="shared" si="10"/>
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="65"/>
-      <c r="C36" s="65">
-        <f>B13</f>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A36" s="55"/>
+      <c r="C36" s="55">
+        <f t="shared" si="8"/>
         <v>63</v>
       </c>
-      <c r="D36" s="65">
-        <f t="shared" si="6"/>
+      <c r="D36" s="55">
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="E36" s="65">
-        <f t="shared" si="7"/>
+      <c r="E36" s="55">
+        <f t="shared" si="10"/>
         <v>1.5873015873015872E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="45" t="s">
         <v>14</v>
       </c>
@@ -4691,9 +5066,9 @@
       </c>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="51">
-        <f t="shared" ref="A40:A47" si="8">A6</f>
+        <f t="shared" ref="A40:A47" si="11">A6</f>
         <v>0</v>
       </c>
       <c r="B40" s="13">
@@ -4709,7 +5084,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="51">
-        <f t="shared" ref="E40:E47" si="9">B6</f>
+        <f t="shared" ref="E40:E47" si="12">B6</f>
         <v>19</v>
       </c>
       <c r="F40" s="13">
@@ -4722,237 +5097,237 @@
       </c>
       <c r="H40" s="5"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="B41" s="13">
-        <f t="shared" ref="B41:B47" si="10">A41^2</f>
+        <f t="shared" ref="B41:B47" si="13">A41^2</f>
         <v>1</v>
       </c>
       <c r="C41" s="13">
-        <f t="shared" ref="C41:C47" si="11">A41^3</f>
+        <f t="shared" ref="C41:C47" si="14">A41^3</f>
         <v>1</v>
       </c>
       <c r="D41" s="13">
-        <f t="shared" ref="D41:D47" si="12">A41^4</f>
+        <f t="shared" ref="D41:D47" si="15">A41^4</f>
         <v>1</v>
       </c>
       <c r="E41" s="51">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>21</v>
       </c>
       <c r="F41" s="13">
-        <f t="shared" ref="F41:F47" si="13">A41*E41</f>
+        <f t="shared" ref="F41:F47" si="16">A41*E41</f>
         <v>21</v>
       </c>
       <c r="G41" s="13">
-        <f t="shared" ref="G41:G47" si="14">B41*E41</f>
+        <f t="shared" ref="G41:G47" si="17">B41*E41</f>
         <v>21</v>
       </c>
       <c r="H41" s="5"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="B42" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="C42" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="D42" s="13">
+        <f t="shared" si="15"/>
+        <v>16</v>
+      </c>
+      <c r="E42" s="51">
         <f t="shared" si="12"/>
-        <v>16</v>
-      </c>
-      <c r="E42" s="51">
-        <f t="shared" si="9"/>
         <v>23</v>
       </c>
       <c r="F42" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>46</v>
       </c>
       <c r="G42" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>92</v>
       </c>
       <c r="H42" s="5"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="B43" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="C43" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>27</v>
       </c>
       <c r="D43" s="13">
+        <f t="shared" si="15"/>
+        <v>81</v>
+      </c>
+      <c r="E43" s="51">
         <f t="shared" si="12"/>
-        <v>81</v>
-      </c>
-      <c r="E43" s="51">
-        <f t="shared" si="9"/>
         <v>28</v>
       </c>
       <c r="F43" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>84</v>
       </c>
       <c r="G43" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>252</v>
       </c>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A44" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="B44" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>16</v>
       </c>
       <c r="C44" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>64</v>
       </c>
       <c r="D44" s="13">
+        <f t="shared" si="15"/>
+        <v>256</v>
+      </c>
+      <c r="E44" s="51">
         <f t="shared" si="12"/>
-        <v>256</v>
-      </c>
-      <c r="E44" s="51">
-        <f t="shared" si="9"/>
         <v>33</v>
       </c>
       <c r="F44" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>132</v>
       </c>
       <c r="G44" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>528</v>
       </c>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="B45" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="C45" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>125</v>
       </c>
       <c r="D45" s="13">
+        <f t="shared" si="15"/>
+        <v>625</v>
+      </c>
+      <c r="E45" s="51">
         <f t="shared" si="12"/>
-        <v>625</v>
-      </c>
-      <c r="E45" s="51">
-        <f t="shared" si="9"/>
         <v>46</v>
       </c>
       <c r="F45" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>230</v>
       </c>
       <c r="G45" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1150</v>
       </c>
       <c r="H45" s="5"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="B46" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>36</v>
       </c>
       <c r="C46" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>216</v>
       </c>
       <c r="D46" s="13">
+        <f t="shared" si="15"/>
+        <v>1296</v>
+      </c>
+      <c r="E46" s="51">
         <f t="shared" si="12"/>
-        <v>1296</v>
-      </c>
-      <c r="E46" s="51">
-        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="F46" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>360</v>
       </c>
       <c r="G46" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>2160</v>
       </c>
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B47" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>49</v>
       </c>
       <c r="C47" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>343</v>
       </c>
       <c r="D47" s="13">
+        <f t="shared" si="15"/>
+        <v>2401</v>
+      </c>
+      <c r="E47" s="51">
         <f t="shared" si="12"/>
-        <v>2401</v>
-      </c>
-      <c r="E47" s="51">
-        <f t="shared" si="9"/>
         <v>63</v>
       </c>
       <c r="F47" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>441</v>
       </c>
       <c r="G47" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3087</v>
       </c>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48" s="52">
         <v>8</v>
       </c>
       <c r="B48" s="13">
-        <f t="shared" ref="B48" si="15">A48^2</f>
+        <f t="shared" ref="B48" si="18">A48^2</f>
         <v>64</v>
       </c>
       <c r="C48" s="13">
-        <f t="shared" ref="C48" si="16">A48^3</f>
+        <f t="shared" ref="C48" si="19">A48^3</f>
         <v>512</v>
       </c>
       <c r="D48" s="13">
-        <f t="shared" ref="D48" si="17">A48^4</f>
+        <f t="shared" ref="D48" si="20">A48^4</f>
         <v>4096</v>
       </c>
       <c r="E48" s="51">
@@ -4960,42 +5335,42 @@
         <v>293</v>
       </c>
       <c r="F48" s="13">
-        <f t="shared" ref="F48" si="18">A48*E48</f>
+        <f t="shared" ref="F48" si="21">A48*E48</f>
         <v>2344</v>
       </c>
       <c r="G48" s="13">
-        <f t="shared" ref="G48" si="19">B48*E48</f>
+        <f t="shared" ref="G48" si="22">B48*E48</f>
         <v>18752</v>
       </c>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="53">
-        <f t="shared" ref="A49:G49" si="20">SUM(A40:A47)</f>
+        <f t="shared" ref="A49:G49" si="23">SUM(A40:A47)</f>
         <v>28</v>
       </c>
       <c r="B49" s="54">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>140</v>
       </c>
       <c r="C49" s="54">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>784</v>
       </c>
       <c r="D49" s="54">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>4676</v>
       </c>
       <c r="E49" s="54">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>293</v>
       </c>
       <c r="F49" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>1314</v>
       </c>
       <c r="G49" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>7290</v>
       </c>
       <c r="H49" s="5"/>
@@ -5016,22 +5391,22 @@
       <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="63" t="s">
+      <c r="A51" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B51" s="63"/>
-      <c r="C51" s="63"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="64"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
-      <c r="I51" s="55"/>
-      <c r="J51" s="55"/>
-      <c r="K51" s="55"/>
-      <c r="L51" s="55"/>
-      <c r="M51" s="55"/>
-      <c r="N51" s="55"/>
+      <c r="I51" s="56"/>
+      <c r="J51" s="56"/>
+      <c r="K51" s="56"/>
+      <c r="L51" s="56"/>
+      <c r="M51" s="56"/>
+      <c r="N51" s="56"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="14">
@@ -5054,12 +5429,12 @@
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
-      <c r="I52" s="56"/>
-      <c r="J52" s="56"/>
-      <c r="K52" s="56"/>
-      <c r="L52" s="56"/>
-      <c r="M52" s="56"/>
-      <c r="N52" s="56"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="57"/>
+      <c r="L52" s="57"/>
+      <c r="M52" s="57"/>
+      <c r="N52" s="57"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="18">
@@ -5106,18 +5481,18 @@
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="57" t="s">
+      <c r="A55" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="B55" s="57"/>
+      <c r="B55" s="58"/>
       <c r="C55" s="5"/>
-      <c r="D55" s="58" t="s">
+      <c r="D55" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="E55" s="58"/>
-      <c r="F55" s="58"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58"/>
+      <c r="E55" s="59"/>
+      <c r="F55" s="59"/>
+      <c r="G55" s="59"/>
+      <c r="H55" s="59"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="28">

</xml_diff>